<commit_message>
A2A and D2D Booking completed 17th march
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/D2D_Booking.xlsx
+++ b/src/main/java/com/crm/qa/testdata/D2D_Booking.xlsx
@@ -9,13 +9,35 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" tabRatio="918" firstSheet="22" activeTab="25"/>
   </bookViews>
   <sheets>
-    <sheet name="WH_2_WH TC3" sheetId="1" r:id="rId1"/>
+    <sheet name="PrePaid_WH_2_WH TC3" sheetId="1" r:id="rId1"/>
     <sheet name="WH_2_WH (GEN) TC4" sheetId="2" r:id="rId2"/>
-    <sheet name="WH_2_WH (POMail) TC5" sheetId="3" r:id="rId3"/>
-    <sheet name="WH_2_WH (WLK) TC6" sheetId="4" r:id="rId4"/>
+    <sheet name="PrePaid_WH_2_WH (POMail) TC5" sheetId="3" r:id="rId3"/>
+    <sheet name="PrePaid_WH_2_WH (WLK) TC6" sheetId="4" r:id="rId4"/>
+    <sheet name="Prepaid_singl_leg TC7" sheetId="5" r:id="rId5"/>
+    <sheet name="Prepaid_singl_leg_Pomail TC8" sheetId="6" r:id="rId6"/>
+    <sheet name="Prepaid_singl_leg_WLK TC9" sheetId="7" r:id="rId7"/>
+    <sheet name="Prepaid_Dub_leg_Gen TC10" sheetId="8" r:id="rId8"/>
+    <sheet name="Prepaid_Dub_leg_POMail TC11" sheetId="9" r:id="rId9"/>
+    <sheet name="Prepaid_Dub_leg_WLK TC12" sheetId="10" r:id="rId10"/>
+    <sheet name="Prepaid_Dub_leg_Gen_wh2wh TC13" sheetId="11" r:id="rId11"/>
+    <sheet name="Prepaid_Dub_legPomai_wh2wh TC14" sheetId="12" r:id="rId12"/>
+    <sheet name="Prepaid_Dub_leg_WLK_wh2wh TC15" sheetId="13" r:id="rId13"/>
+    <sheet name="PostPaid_WH_2_WH TC16" sheetId="14" r:id="rId14"/>
+    <sheet name="PostPaid_WH_2_WH (GEN) TC17" sheetId="15" r:id="rId15"/>
+    <sheet name="PostPaid_WH_2_WH (POMail) TC18" sheetId="16" r:id="rId16"/>
+    <sheet name="PostPaid_WH_2_WH (WLK) TC19" sheetId="17" r:id="rId17"/>
+    <sheet name="Postpaid_singl_leg TC20" sheetId="18" r:id="rId18"/>
+    <sheet name="Postpaid_singl_leg_Pomail TC21" sheetId="19" r:id="rId19"/>
+    <sheet name="Postpaid_singl_leg_WLK TC22" sheetId="20" r:id="rId20"/>
+    <sheet name="Postpaid_Dub_leg_Gen TC23" sheetId="21" r:id="rId21"/>
+    <sheet name="Postpaid_Dub_leg_POMail TC24" sheetId="22" r:id="rId22"/>
+    <sheet name="Postpaid_Dub_leg_WLK TC25" sheetId="23" r:id="rId23"/>
+    <sheet name="Postpaid_Dub_leg_Gen_wh2wh TC26" sheetId="24" r:id="rId24"/>
+    <sheet name="Pospaid_Dub_legPomai_wh2wh TC27" sheetId="25" r:id="rId25"/>
+    <sheet name="Postpaid_Dub_leg_WLK_wh2wh TC28" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="39">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -112,6 +134,39 @@
   <si>
     <t>WLKDL1DD</t>
   </si>
+  <si>
+    <t>Flight</t>
+  </si>
+  <si>
+    <t>Via</t>
+  </si>
+  <si>
+    <t>CCU</t>
+  </si>
+  <si>
+    <t>Via_WH</t>
+  </si>
+  <si>
+    <t>Via Flight</t>
+  </si>
+  <si>
+    <t>Via_Des_WH</t>
+  </si>
+  <si>
+    <t>BO2</t>
+  </si>
+  <si>
+    <t>GG1</t>
+  </si>
+  <si>
+    <t>Des Airport</t>
+  </si>
+  <si>
+    <t>LAVDL1DD</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
 </sst>
 </file>
 
@@ -152,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -167,6 +222,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,10 +505,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,8 +635,1406 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -703,12 +2162,1033 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +3256,7 @@
         <v>20</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -792,10 +3272,10 @@
       <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -819,12 +3299,8 @@
       <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -834,10 +3310,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,4 +3438,689 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>